<commit_message>
Updated Version of MultiFreq
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server1\Desktop\NVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="LocalStiffness" sheetId="1" r:id="rId1"/>
     <sheet name="Torque_rpm" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>local stiffness at mount 1</t>
   </si>
@@ -58,12 +58,15 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>freq(rpm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,10 +99,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -385,12 +388,12 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
@@ -405,73 +408,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="O1" s="3" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
       <c r="O2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3" t="s">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -531,7 +534,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="B4">
         <v>10000000</v>
@@ -596,7 +599,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>15</v>
+        <v>750</v>
       </c>
       <c r="B5">
         <v>10000000</v>
@@ -661,7 +664,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="B6">
         <v>10000000</v>
@@ -726,7 +729,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>25</v>
+        <v>1250</v>
       </c>
       <c r="B7">
         <v>10000000</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>30</v>
+        <v>1500</v>
       </c>
       <c r="B8">
         <v>10000000</v>

</xml_diff>